<commit_message>
update all the data files
</commit_message>
<xml_diff>
--- a/data/dac-train.xlsx
+++ b/data/dac-train.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E101"/>
+  <dimension ref="A1:D100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,16 +454,11 @@
           <t>Param2</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Param3</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Zelda--param1-00.38--1-22 A King's Request.dac</t>
+          <t>Zelda--param1-00.79--1-40.dac</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -472,15 +467,16 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.38</v>
-      </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
+        <v>0.79</v>
+      </c>
+      <c r="D2" t="n">
+        <v>40</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Zelda--param1-00.26--2-25 Mipha's Role.dac</t>
+          <t>Zelda--param1-00.02--5-14.dac</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -489,15 +485,16 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.26</v>
-      </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
+        <v>0.02</v>
+      </c>
+      <c r="D3" t="n">
+        <v>14</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Zelda--param1-00.37--2-21 Waterblight Ganon Appears.dac</t>
+          <t>Zelda--param1-00.65--3-20.dac</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -506,15 +503,16 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.37</v>
-      </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
+        <v>0.65</v>
+      </c>
+      <c r="D4" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Zelda--param1-00.94--1-38 Hateno Ancient Tech Lab.dac</t>
+          <t>Zelda--param1-00.03--3-19.dac</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -523,15 +521,16 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.9399999999999999</v>
-      </c>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
+        <v>0.03</v>
+      </c>
+      <c r="D5" t="n">
+        <v>19</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Zelda--param1-00.46--1-09 The Beast.dac</t>
+          <t>Zelda--param1-00.51--6-05.dac</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -540,15 +539,16 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.46</v>
-      </c>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
+        <v>0.51</v>
+      </c>
+      <c r="D6" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Zelda--param1-00.90--2-33 Malanya's Theme.dac</t>
+          <t>Zelda--param1-00.25--6-12.dac</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -557,15 +557,16 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
+        <v>0.25</v>
+      </c>
+      <c r="D7" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Zelda--param1-00.94--3-26 Tarrey Town.dac</t>
+          <t>Zelda--param1-00.27--3-29.dac</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -574,15 +575,16 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.9399999999999999</v>
-      </c>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
+        <v>0.27</v>
+      </c>
+      <c r="D8" t="n">
+        <v>29</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Zelda--param1-00.45--4-04 The Great Deku Tree.dac</t>
+          <t>Zelda--param1-00.87--1-31.dac</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -591,15 +593,16 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.45</v>
-      </c>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
+        <v>0.87</v>
+      </c>
+      <c r="D9" t="n">
+        <v>31</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Zelda--param1-00.96--2-32 Malanya's Theme.dac</t>
+          <t>Zelda--param1-00.30--4-14.dac</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -608,15 +611,16 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.96</v>
-      </c>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
+        <v>0.3</v>
+      </c>
+      <c r="D10" t="n">
+        <v>14</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Zelda--param1-00.89--1-35 Dye Clothes - Coloring.dac</t>
+          <t>Zelda--param1-00.15--2-10.dac</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -625,15 +629,16 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.89</v>
-      </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
+        <v>0.15</v>
+      </c>
+      <c r="D11" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Zelda--param1-00.28--4-08 Hestu's Dance.dac</t>
+          <t>Zelda--param1-00.77--4-23.dac</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -642,15 +647,16 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.28</v>
-      </c>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
+        <v>0.77</v>
+      </c>
+      <c r="D12" t="n">
+        <v>23</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Zelda--param1-00.36--5-13 Windblight Ganon Appears.dac</t>
+          <t>Zelda--param1-00.06--1-04.dac</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -659,15 +665,16 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.36</v>
-      </c>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
+        <v>0.06</v>
+      </c>
+      <c r="D13" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Zelda--param1-00.49--1-19 Heart Container-Stamina Vessel Get.dac</t>
+          <t>Zelda--param1-00.83--6-11.dac</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -676,15 +683,16 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.49</v>
-      </c>
-      <c r="D14" t="inlineStr"/>
-      <c r="E14" t="inlineStr"/>
+        <v>0.83</v>
+      </c>
+      <c r="D14" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Zelda--param1-00.59--2-32 Lurelin Village (Night).dac</t>
+          <t>Zelda--param1-00.35.dac</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -693,15 +701,14 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.59</v>
+        <v>0.35</v>
       </c>
       <c r="D15" t="inlineStr"/>
-      <c r="E15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Zelda--param1-00.06--1-04 Field (Day).dac</t>
+          <t>Zelda--param1-00.39--3-06.dac</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -710,15 +717,16 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0.06</v>
-      </c>
-      <c r="D16" t="inlineStr"/>
-      <c r="E16" t="inlineStr"/>
+        <v>0.39</v>
+      </c>
+      <c r="D16" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Zelda--param1-00.30--4-02 Korok Forest - Day.dac</t>
+          <t>Zelda--param1-00.22--1-32.dac</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -727,15 +735,16 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="D17" t="inlineStr"/>
-      <c r="E17" t="inlineStr"/>
+        <v>0.22</v>
+      </c>
+      <c r="D17" t="n">
+        <v>32</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Zelda--param1-00.17--3-30 Parasail Course.dac</t>
+          <t>Zelda--param1-00.83--2-35.dac</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -744,15 +753,16 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.17</v>
-      </c>
-      <c r="D18" t="inlineStr"/>
-      <c r="E18" t="inlineStr"/>
+        <v>0.83</v>
+      </c>
+      <c r="D18" t="n">
+        <v>35</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Zelda--param1-00.07--3-01 Gerudo Canyon.dac</t>
+          <t>Zelda--param1-00.95--2-26.dac</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -761,15 +771,16 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0.07000000000000001</v>
-      </c>
-      <c r="D19" t="inlineStr"/>
-      <c r="E19" t="inlineStr"/>
+        <v>0.95</v>
+      </c>
+      <c r="D19" t="n">
+        <v>26</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Zelda--param1-00.25--2-34 Lord of the Mountain.dac</t>
+          <t>Zelda--param1-00.52--3-04.dac</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -778,15 +789,16 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="D20" t="inlineStr"/>
-      <c r="E20" t="inlineStr"/>
+        <v>0.52</v>
+      </c>
+      <c r="D20" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Zelda--param1-00.79--1-40 Combat Trial.dac</t>
+          <t>Zelda--param1-00.72--4-18.dac</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -795,1370 +807,1275 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0.79</v>
-      </c>
-      <c r="D21" t="inlineStr"/>
-      <c r="E21" t="inlineStr"/>
+        <v>0.72</v>
+      </c>
+      <c r="D21" t="n">
+        <v>18</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>8bit--param1-00.06.dac</t>
+          <t>lofi--param1-00.74.dac</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>8bit</t>
+          <t>lofi</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0.06</v>
+        <v>0.74</v>
       </c>
       <c r="D22" t="inlineStr"/>
-      <c r="E22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>8bit--param1-00.70.dac</t>
+          <t>lofi--param1-00.54.dac</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>8bit</t>
+          <t>lofi</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0.7</v>
+        <v>0.54</v>
       </c>
       <c r="D23" t="inlineStr"/>
-      <c r="E23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>8bit--param1-00.71--46 Dark Genie Final Form.dac</t>
+          <t>lofi--param1-00.38.dac</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>8bit</t>
+          <t>lofi</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.71</v>
+        <v>0.38</v>
       </c>
       <c r="D24" t="inlineStr"/>
-      <c r="E24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>8bit--param1-00.73--42 Time of Destiny.dac</t>
+          <t>lofi--param1-00.60--Cymatics.dac</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>8bit</t>
+          <t>lofi</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0.73</v>
+        <v>0.6</v>
       </c>
       <c r="D25" t="inlineStr"/>
-      <c r="E25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>8bit--param1-00.85.dac</t>
+          <t>lofi--param1-00.91.dac</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>8bit</t>
+          <t>lofi</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0.85</v>
+        <v>0.91</v>
       </c>
       <c r="D26" t="inlineStr"/>
-      <c r="E26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>8bit--param1-00.71--31 Emergency.dac</t>
+          <t>lofi--param1-00.62--Cymatics.dac</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>8bit</t>
+          <t>lofi</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>0.71</v>
+        <v>0.62</v>
       </c>
       <c r="D27" t="inlineStr"/>
-      <c r="E27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>8bit--param1-00.81.dac</t>
+          <t>lofi--param1-00.93.dac</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>8bit</t>
+          <t>lofi</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.93</v>
       </c>
       <c r="D28" t="inlineStr"/>
-      <c r="E28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>8bit--param1-00.62--01 Dark Cloud Main Theme.dac</t>
+          <t>lofi--param1-00.25--Cymatics.dac</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>8bit</t>
+          <t>lofi</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>0.62</v>
+        <v>0.25</v>
       </c>
       <c r="D29" t="inlineStr"/>
-      <c r="E29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>8bit--param1-00.34.dac</t>
+          <t>lofi--param1-00.22.dac</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>8bit</t>
+          <t>lofi</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>0.34</v>
+        <v>0.22</v>
       </c>
       <c r="D30" t="inlineStr"/>
-      <c r="E30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>8bit--param1-00.78--33 Land Of Hope.dac</t>
+          <t>lofi--param1-00.14.dac</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>8bit</t>
+          <t>lofi</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0.78</v>
+        <v>0.14</v>
       </c>
       <c r="D31" t="inlineStr"/>
-      <c r="E31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>8bit--param1-00.07.dac</t>
+          <t>lofi--param1-00.06.dac</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>8bit</t>
+          <t>lofi</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.06</v>
       </c>
       <c r="D32" t="inlineStr"/>
-      <c r="E32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>8bit--param1-00.14.dac</t>
+          <t>lofi--param1-00.92.dac</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>8bit</t>
+          <t>lofi</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>0.14</v>
+        <v>0.92</v>
       </c>
       <c r="D33" t="inlineStr"/>
-      <c r="E33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>8bit--param1-00.90.dac</t>
+          <t>lofi--param1-00.50.dac</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>8bit</t>
+          <t>lofi</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="D34" t="inlineStr"/>
-      <c r="E34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>8bit--param1-00.88.dac</t>
+          <t>lofi--param1-00.02.dac</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>8bit</t>
+          <t>lofi</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>0.88</v>
+        <v>0.02</v>
       </c>
       <c r="D35" t="inlineStr"/>
-      <c r="E35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>8bit--param1-00.15--43 Gallery of Time.dac</t>
+          <t>lofi--param1-00.01.dac</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>8bit</t>
+          <t>lofi</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>0.15</v>
+        <v>0.01</v>
       </c>
       <c r="D36" t="inlineStr"/>
-      <c r="E36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>8bit--param1-00.54.dac</t>
+          <t>lofi--param1-00.20.dac</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>8bit</t>
+          <t>lofi</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>0.54</v>
+        <v>0.2</v>
       </c>
       <c r="D37" t="inlineStr"/>
-      <c r="E37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>8bit--param1-00.78--12 Divine Beast Cave.dac</t>
+          <t>lofi--param1-01.00.dac</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>8bit</t>
+          <t>lofi</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>0.78</v>
+        <v>1</v>
       </c>
       <c r="D38" t="inlineStr"/>
-      <c r="E38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>8bit--param1-00.26.dac</t>
+          <t>lofi--param1-00.18.dac</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>8bit</t>
+          <t>lofi</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>0.26</v>
+        <v>0.18</v>
       </c>
       <c r="D39" t="inlineStr"/>
-      <c r="E39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>8bit--param1-00.49.dac</t>
+          <t>lofi--param1-00.35.dac</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>8bit</t>
+          <t>lofi</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>0.49</v>
+        <v>0.35</v>
       </c>
       <c r="D40" t="inlineStr"/>
-      <c r="E40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>8bit--param1-00.67--19 Legend of Hunter.dac</t>
+          <t>Fusion--param1-00.25.dac</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>8bit</t>
+          <t>Fusion</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>0.67</v>
+        <v>0.25</v>
       </c>
       <c r="D41" t="inlineStr"/>
-      <c r="E41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>duduk--param1-00.85.dac</t>
+          <t>Fusion--param1-00.65.dac</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>duduk</t>
+          <t>Fusion</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>0.85</v>
+        <v>0.65</v>
       </c>
       <c r="D42" t="inlineStr"/>
-      <c r="E42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>duduk--param1-00.70.dac</t>
+          <t>Fusion--param1-00.40.dac</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>duduk</t>
+          <t>Fusion</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>0.7</v>
+        <v>0.4</v>
       </c>
       <c r="D43" t="inlineStr"/>
-      <c r="E43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>duduk--param1-00.38.dac</t>
+          <t>Fusion--param1-00.22.dac</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>duduk</t>
+          <t>Fusion</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>0.38</v>
+        <v>0.22</v>
       </c>
       <c r="D44" t="inlineStr"/>
-      <c r="E44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>duduk--param1-00.76.dac</t>
+          <t>Fusion--param1-00.09.dac</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>duduk</t>
+          <t>Fusion</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>0.76</v>
+        <v>0.09</v>
       </c>
       <c r="D45" t="inlineStr"/>
-      <c r="E45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>duduk--param1-00.55.dac</t>
+          <t>Fusion--param1-00.96--segment_03..dac</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>duduk</t>
+          <t>Fusion</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>0.55</v>
+        <v>0.96</v>
       </c>
       <c r="D46" t="inlineStr"/>
-      <c r="E46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>duduk--param1-00.23.dac</t>
+          <t>Fusion--param1-00.24.dac</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>duduk</t>
+          <t>Fusion</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>0.23</v>
+        <v>0.24</v>
       </c>
       <c r="D47" t="inlineStr"/>
-      <c r="E47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>duduk--param1-00.11.dac</t>
+          <t>Fusion--param1-00.20.dac</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>duduk</t>
+          <t>Fusion</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>0.11</v>
+        <v>0.2</v>
       </c>
       <c r="D48" t="inlineStr"/>
-      <c r="E48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>duduk--param1-00.67.dac</t>
+          <t>Fusion--param1-00.51.dac</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>duduk</t>
+          <t>Fusion</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>0.67</v>
+        <v>0.51</v>
       </c>
       <c r="D49" t="inlineStr"/>
-      <c r="E49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>duduk--param1-00.63.dac</t>
+          <t>Fusion--param1-00.27.dac</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>duduk</t>
+          <t>Fusion</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>0.63</v>
+        <v>0.27</v>
       </c>
       <c r="D50" t="inlineStr"/>
-      <c r="E50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>duduk--param1-00.51.dac</t>
+          <t>Fusion--param1-00.78.dac</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>duduk</t>
+          <t>Fusion</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>0.51</v>
+        <v>0.78</v>
       </c>
       <c r="D51" t="inlineStr"/>
-      <c r="E51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>duduk--param1-00.02.dac</t>
+          <t>Fusion--param1-00.11.dac</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>duduk</t>
+          <t>Fusion</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>0.02</v>
+        <v>0.11</v>
       </c>
       <c r="D52" t="inlineStr"/>
-      <c r="E52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>duduk--param1-00.66.dac</t>
+          <t>Fusion--param1-00.45.dac</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>duduk</t>
+          <t>Fusion</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>0.66</v>
+        <v>0.45</v>
       </c>
       <c r="D53" t="inlineStr"/>
-      <c r="E53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>duduk--param1-00.77.dac</t>
+          <t>Fusion--param1-00.37.dac</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>duduk</t>
+          <t>Fusion</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>0.77</v>
+        <v>0.37</v>
       </c>
       <c r="D54" t="inlineStr"/>
-      <c r="E54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>duduk--param1-00.88.dac</t>
+          <t>Fusion--param1-00.92--segment_09..dac</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>duduk</t>
+          <t>Fusion</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>0.88</v>
+        <v>0.92</v>
       </c>
       <c r="D55" t="inlineStr"/>
-      <c r="E55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>duduk--param1-00.54--KSHMR_Duduk_19_One_Shot_F#m.dac</t>
+          <t>Fusion--param1-00.79.dac</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>duduk</t>
+          <t>Fusion</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>0.54</v>
+        <v>0.79</v>
       </c>
       <c r="D56" t="inlineStr"/>
-      <c r="E56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>duduk--param1-00.30.dac</t>
+          <t>Fusion--param1-00.34--segment_03..dac</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>duduk</t>
+          <t>Fusion</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>0.3</v>
+        <v>0.34</v>
       </c>
       <c r="D57" t="inlineStr"/>
-      <c r="E57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>duduk--param1-00.80.dac</t>
+          <t>Fusion--param1-00.42.dac</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>duduk</t>
+          <t>Fusion</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>0.8</v>
+        <v>0.42</v>
       </c>
       <c r="D58" t="inlineStr"/>
-      <c r="E58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>duduk--param1-00.54--KSHMR_Duduk_14_One_Shot_Fm.dac</t>
+          <t>Fusion--param1-00.53.dac</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>duduk</t>
+          <t>Fusion</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>0.54</v>
+        <v>0.53</v>
       </c>
       <c r="D59" t="inlineStr"/>
-      <c r="E59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>duduk--param1-00.74.dac</t>
+          <t>Fusion--param1-00.82.dac</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>duduk</t>
+          <t>Fusion</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>0.74</v>
+        <v>0.82</v>
       </c>
       <c r="D60" t="inlineStr"/>
-      <c r="E60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>duduk--param1-00.26.dac</t>
+          <t>8bit--param1-00.19--40.dac</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>duduk</t>
+          <t>8bit</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>0.26</v>
+        <v>0.19</v>
       </c>
       <c r="D61" t="inlineStr"/>
-      <c r="E61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>lofi--param1-00.49.dac</t>
+          <t>8bit--param1-00.62--23.dac</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>lofi</t>
+          <t>8bit</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>0.49</v>
+        <v>0.62</v>
       </c>
       <c r="D62" t="inlineStr"/>
-      <c r="E62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>lofi--param1-00.14.dac</t>
+          <t>8bit--param1-00.81.dac</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>lofi</t>
+          <t>8bit</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>0.14</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="D63" t="inlineStr"/>
-      <c r="E63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>lofi--param1-00.25--Cymatics - Lofi Melody Loop 17 - 120 BPM F# Maj.dac</t>
+          <t>8bit--param1-00.01.dac</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>lofi</t>
+          <t>8bit</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>0.25</v>
+        <v>0.01</v>
       </c>
       <c r="D64" t="inlineStr"/>
-      <c r="E64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>lofi--param1-00.38.dac</t>
+          <t>8bit--param1-00.50.dac</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>lofi</t>
+          <t>8bit</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>0.38</v>
+        <v>0.5</v>
       </c>
       <c r="D65" t="inlineStr"/>
-      <c r="E65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>lofi--param1-00.18.dac</t>
+          <t>8bit--param1-00.55.dac</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>lofi</t>
+          <t>8bit</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>0.18</v>
+        <v>0.55</v>
       </c>
       <c r="D66" t="inlineStr"/>
-      <c r="E66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>lofi--param1-00.92.dac</t>
+          <t>8bit--param1-00.85.dac</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>lofi</t>
+          <t>8bit</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>0.92</v>
+        <v>0.85</v>
       </c>
       <c r="D67" t="inlineStr"/>
-      <c r="E67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>lofi--param1-00.06.dac</t>
+          <t>8bit--param1-00.71--31.dac</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>lofi</t>
+          <t>8bit</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>0.06</v>
+        <v>0.71</v>
       </c>
       <c r="D68" t="inlineStr"/>
-      <c r="E68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>lofi--param1-00.50.dac</t>
+          <t>8bit--param1-00.15--43.dac</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>lofi</t>
+          <t>8bit</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="D69" t="inlineStr"/>
-      <c r="E69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>lofi--param1-00.25--Cymatics - Lofi Melody Loop 10 - 90 BPM B Min.dac</t>
+          <t>8bit--param1-00.60.dac</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>lofi</t>
+          <t>8bit</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>0.25</v>
+        <v>0.6</v>
       </c>
       <c r="D70" t="inlineStr"/>
-      <c r="E70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>lofi--param1-00.44.dac</t>
+          <t>8bit--param1-00.06.dac</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>lofi</t>
+          <t>8bit</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>0.44</v>
+        <v>0.06</v>
       </c>
       <c r="D71" t="inlineStr"/>
-      <c r="E71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>lofi--param1-00.35.dac</t>
+          <t>8bit--param1-00.14.dac</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>lofi</t>
+          <t>8bit</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>0.35</v>
+        <v>0.14</v>
       </c>
       <c r="D72" t="inlineStr"/>
-      <c r="E72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>lofi--param1-00.20.dac</t>
+          <t>8bit--param1-00.62--01.dac</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>lofi</t>
+          <t>8bit</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>0.2</v>
+        <v>0.62</v>
       </c>
       <c r="D73" t="inlineStr"/>
-      <c r="E73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>lofi--param1-00.88.dac</t>
+          <t>8bit--param1-00.88.dac</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>lofi</t>
+          <t>8bit</t>
         </is>
       </c>
       <c r="C74" t="n">
         <v>0.88</v>
       </c>
       <c r="D74" t="inlineStr"/>
-      <c r="E74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>lofi--param1-00.81.dac</t>
+          <t>8bit--param1-00.82.dac</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>lofi</t>
+          <t>8bit</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.82</v>
       </c>
       <c r="D75" t="inlineStr"/>
-      <c r="E75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>lofi--param1-00.01.dac</t>
+          <t>8bit--param1-00.67--19.dac</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>lofi</t>
+          <t>8bit</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>0.01</v>
+        <v>0.67</v>
       </c>
       <c r="D76" t="inlineStr"/>
-      <c r="E76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>lofi--param1-01.00.dac</t>
+          <t>8bit--param1-00.49.dac</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>lofi</t>
+          <t>8bit</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>1</v>
+        <v>0.49</v>
       </c>
       <c r="D77" t="inlineStr"/>
-      <c r="E77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>lofi--param1-00.93.dac</t>
+          <t>8bit--param1-00.40.dac</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>lofi</t>
+          <t>8bit</t>
         </is>
       </c>
       <c r="C78" t="n">
-        <v>0.93</v>
+        <v>0.4</v>
       </c>
       <c r="D78" t="inlineStr"/>
-      <c r="E78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>lofi--param1-00.74.dac</t>
+          <t>8bit--param1-00.71--46.dac</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>lofi</t>
+          <t>8bit</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>0.74</v>
+        <v>0.71</v>
       </c>
       <c r="D79" t="inlineStr"/>
-      <c r="E79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>lofi--param1-00.91.dac</t>
+          <t>8bit--param1-00.12.dac</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>lofi</t>
+          <t>8bit</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>0.91</v>
+        <v>0.12</v>
       </c>
       <c r="D80" t="inlineStr"/>
-      <c r="E80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>lofi--param1-00.54.dac</t>
+          <t>duduk--param1-00.22.dac</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>lofi</t>
+          <t>duduk</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>0.54</v>
+        <v>0.22</v>
       </c>
       <c r="D81" t="inlineStr"/>
-      <c r="E81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Fusion--param1-00.37.dac</t>
+          <t>duduk--param1-00.51.dac</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Fusion</t>
+          <t>duduk</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>0.37</v>
+        <v>0.51</v>
       </c>
       <c r="D82" t="inlineStr"/>
-      <c r="E82" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Fusion--param1-00.11.dac</t>
+          <t>duduk--param1-00.77.dac</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Fusion</t>
+          <t>duduk</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>0.11</v>
+        <v>0.77</v>
       </c>
       <c r="D83" t="inlineStr"/>
-      <c r="E83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Fusion--param1-00.96--segment_03. All Gods With Me.dac</t>
+          <t>duduk--param1-00.85.dac</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Fusion</t>
+          <t>duduk</t>
         </is>
       </c>
       <c r="C84" t="n">
-        <v>0.96</v>
+        <v>0.85</v>
       </c>
       <c r="D84" t="inlineStr"/>
-      <c r="E84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Fusion--param1-00.76.dac</t>
+          <t>duduk--param1-00.70.dac</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Fusion</t>
+          <t>duduk</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>0.76</v>
+        <v>0.7</v>
       </c>
       <c r="D85" t="inlineStr"/>
-      <c r="E85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Fusion--param1-00.42.dac</t>
+          <t>duduk--param1-00.11.dac</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Fusion</t>
+          <t>duduk</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>0.42</v>
+        <v>0.11</v>
       </c>
       <c r="D86" t="inlineStr"/>
-      <c r="E86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Fusion--param1-00.09.dac</t>
+          <t>duduk--param1-00.38.dac</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Fusion</t>
+          <t>duduk</t>
         </is>
       </c>
       <c r="C87" t="n">
-        <v>0.09</v>
+        <v>0.38</v>
       </c>
       <c r="D87" t="inlineStr"/>
-      <c r="E87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Fusion--param1-00.39.dac</t>
+          <t>duduk--param1-00.55.dac</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Fusion</t>
+          <t>duduk</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>0.39</v>
+        <v>0.55</v>
       </c>
       <c r="D88" t="inlineStr"/>
-      <c r="E88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Fusion--param1-00.41.dac</t>
+          <t>duduk--param1-00.66.dac</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Fusion</t>
+          <t>duduk</t>
         </is>
       </c>
       <c r="C89" t="n">
-        <v>0.41</v>
+        <v>0.66</v>
       </c>
       <c r="D89" t="inlineStr"/>
-      <c r="E89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Fusion--param1-00.92--segment_09. The Chieftain1.dac</t>
+          <t>duduk--param1-00.88.dac</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Fusion</t>
+          <t>duduk</t>
         </is>
       </c>
       <c r="C90" t="n">
-        <v>0.92</v>
+        <v>0.88</v>
       </c>
       <c r="D90" t="inlineStr"/>
-      <c r="E90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Fusion--param1-00.34--segment_01. The End.dac</t>
+          <t>duduk--param1-00.02.dac</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Fusion</t>
+          <t>duduk</t>
         </is>
       </c>
       <c r="C91" t="n">
-        <v>0.34</v>
+        <v>0.02</v>
       </c>
       <c r="D91" t="inlineStr"/>
-      <c r="E91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Fusion--param1-00.82.dac</t>
+          <t>duduk--param1-00.80.dac</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Fusion</t>
+          <t>duduk</t>
         </is>
       </c>
       <c r="C92" t="n">
-        <v>0.82</v>
+        <v>0.8</v>
       </c>
       <c r="D92" t="inlineStr"/>
-      <c r="E92" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Fusion--param1-00.24.dac</t>
+          <t>duduk--param1-00.54--KSHMR_Duduk_14_One_Shot_Fm.dac</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Fusion</t>
+          <t>duduk</t>
         </is>
       </c>
       <c r="C93" t="n">
-        <v>0.24</v>
+        <v>0.54</v>
       </c>
       <c r="D93" t="inlineStr"/>
-      <c r="E93" t="inlineStr"/>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Fusion--param1-00.79.dac</t>
+          <t>duduk--param1-00.26.dac</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Fusion</t>
+          <t>duduk</t>
         </is>
       </c>
       <c r="C94" t="n">
-        <v>0.79</v>
+        <v>0.26</v>
       </c>
       <c r="D94" t="inlineStr"/>
-      <c r="E94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Fusion--param1-00.45.dac</t>
+          <t>duduk--param1-00.58.dac</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Fusion</t>
+          <t>duduk</t>
         </is>
       </c>
       <c r="C95" t="n">
-        <v>0.45</v>
+        <v>0.58</v>
       </c>
       <c r="D95" t="inlineStr"/>
-      <c r="E95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Fusion--param1-00.33.dac</t>
+          <t>duduk--param1-00.63.dac</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Fusion</t>
+          <t>duduk</t>
         </is>
       </c>
       <c r="C96" t="n">
-        <v>0.33</v>
+        <v>0.63</v>
       </c>
       <c r="D96" t="inlineStr"/>
-      <c r="E96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Fusion--param1-00.86.dac</t>
+          <t>duduk--param1-00.23.dac</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Fusion</t>
+          <t>duduk</t>
         </is>
       </c>
       <c r="C97" t="n">
-        <v>0.86</v>
+        <v>0.23</v>
       </c>
       <c r="D97" t="inlineStr"/>
-      <c r="E97" t="inlineStr"/>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Fusion--param1-00.19.dac</t>
+          <t>duduk--param1-00.74.dac</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Fusion</t>
+          <t>duduk</t>
         </is>
       </c>
       <c r="C98" t="n">
-        <v>0.19</v>
+        <v>0.74</v>
       </c>
       <c r="D98" t="inlineStr"/>
-      <c r="E98" t="inlineStr"/>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Fusion--param1-00.78.dac</t>
+          <t>duduk--param1-00.93.dac</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Fusion</t>
+          <t>duduk</t>
         </is>
       </c>
       <c r="C99" t="n">
-        <v>0.78</v>
+        <v>0.93</v>
       </c>
       <c r="D99" t="inlineStr"/>
-      <c r="E99" t="inlineStr"/>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Fusion--param1-00.92--segment_09. The Chieftain.dac</t>
+          <t>duduk--param1-00.76.dac</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Fusion</t>
+          <t>duduk</t>
         </is>
       </c>
       <c r="C100" t="n">
-        <v>0.92</v>
+        <v>0.76</v>
       </c>
       <c r="D100" t="inlineStr"/>
-      <c r="E100" t="inlineStr"/>
-    </row>
-    <row r="101">
-      <c r="A101" t="inlineStr">
-        <is>
-          <t>Fusion--param1-00.51.dac</t>
-        </is>
-      </c>
-      <c r="B101" t="inlineStr">
-        <is>
-          <t>Fusion</t>
-        </is>
-      </c>
-      <c r="C101" t="n">
-        <v>0.51</v>
-      </c>
-      <c r="D101" t="inlineStr"/>
-      <c r="E101" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
update all data folders with renamed files
</commit_message>
<xml_diff>
--- a/data/dac-train.xlsx
+++ b/data/dac-train.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D100"/>
+  <dimension ref="A1:C100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,16 +449,11 @@
           <t>Param1</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Param2</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Zelda--param1-00.79--1-40.dac</t>
+          <t>Zelda--param1-00.11.dac</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -467,16 +462,13 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.79</v>
-      </c>
-      <c r="D2" t="n">
-        <v>40</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Zelda--param1-00.02--5-14.dac</t>
+          <t>Zelda--param1-00.16.dac</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -485,16 +477,13 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="D3" t="n">
-        <v>14</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Zelda--param1-00.65--3-20.dac</t>
+          <t>Zelda--param1-00.19.dac</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -503,16 +492,13 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.65</v>
-      </c>
-      <c r="D4" t="n">
-        <v>20</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Zelda--param1-00.03--3-19.dac</t>
+          <t>Zelda--param1-00.40.dac</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -521,16 +507,13 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.03</v>
-      </c>
-      <c r="D5" t="n">
-        <v>19</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Zelda--param1-00.51--6-05.dac</t>
+          <t>Zelda--param1-00.48.dac</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -539,16 +522,13 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.51</v>
-      </c>
-      <c r="D6" t="n">
-        <v>5</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Zelda--param1-00.25--6-12.dac</t>
+          <t>Zelda--param1-00.03.dac</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -557,16 +537,13 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="D7" t="n">
-        <v>12</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Zelda--param1-00.27--3-29.dac</t>
+          <t>Zelda--param1-00.04.dac</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -575,16 +552,13 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.27</v>
-      </c>
-      <c r="D8" t="n">
-        <v>29</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Zelda--param1-00.87--1-31.dac</t>
+          <t>Zelda--param1-00.30.dac</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -593,16 +567,13 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.87</v>
-      </c>
-      <c r="D9" t="n">
-        <v>31</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Zelda--param1-00.30--4-14.dac</t>
+          <t>Zelda--param1-00.14.dac</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -611,16 +582,13 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="D10" t="n">
-        <v>14</v>
+        <v>0.14</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Zelda--param1-00.15--2-10.dac</t>
+          <t>Zelda--param1-00.18.dac</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -629,16 +597,13 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="D11" t="n">
-        <v>10</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Zelda--param1-00.77--4-23.dac</t>
+          <t>Zelda--param1-00.81.dac</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -647,16 +612,13 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.77</v>
-      </c>
-      <c r="D12" t="n">
-        <v>23</v>
+        <v>0.8100000000000001</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Zelda--param1-00.06--1-04.dac</t>
+          <t>Zelda--param1-00.29.dac</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -665,16 +627,13 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.06</v>
-      </c>
-      <c r="D13" t="n">
-        <v>4</v>
+        <v>0.29</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Zelda--param1-00.83--6-11.dac</t>
+          <t>Zelda--param1-00.59.dac</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -683,16 +642,13 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.83</v>
-      </c>
-      <c r="D14" t="n">
-        <v>11</v>
+        <v>0.59</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Zelda--param1-00.35.dac</t>
+          <t>Zelda--param1-00.34.dac</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -701,14 +657,13 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.35</v>
-      </c>
-      <c r="D15" t="inlineStr"/>
+        <v>0.34</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Zelda--param1-00.39--3-06.dac</t>
+          <t>Zelda--param1-00.75.dac</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -717,16 +672,13 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0.39</v>
-      </c>
-      <c r="D16" t="n">
-        <v>6</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Zelda--param1-00.22--1-32.dac</t>
+          <t>Zelda--param1-00.62.dac</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -735,16 +687,13 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.22</v>
-      </c>
-      <c r="D17" t="n">
-        <v>32</v>
+        <v>0.62</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Zelda--param1-00.83--2-35.dac</t>
+          <t>Zelda--param1-00.67.dac</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -753,16 +702,13 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.83</v>
-      </c>
-      <c r="D18" t="n">
-        <v>35</v>
+        <v>0.67</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Zelda--param1-00.95--2-26.dac</t>
+          <t>Zelda--param1-00.54.dac</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -771,16 +717,13 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0.95</v>
-      </c>
-      <c r="D19" t="n">
-        <v>26</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Zelda--param1-00.52--3-04.dac</t>
+          <t>Zelda--param1-00.87.dac</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -789,16 +732,13 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0.52</v>
-      </c>
-      <c r="D20" t="n">
-        <v>4</v>
+        <v>0.87</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Zelda--param1-00.72--4-18.dac</t>
+          <t>Zelda--param1-00.37.dac</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -807,10 +747,7 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0.72</v>
-      </c>
-      <c r="D21" t="n">
-        <v>18</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="22">
@@ -827,7 +764,6 @@
       <c r="C22" t="n">
         <v>0.74</v>
       </c>
-      <c r="D22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -843,7 +779,6 @@
       <c r="C23" t="n">
         <v>0.54</v>
       </c>
-      <c r="D23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -859,12 +794,11 @@
       <c r="C24" t="n">
         <v>0.38</v>
       </c>
-      <c r="D24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>lofi--param1-00.60--Cymatics.dac</t>
+          <t>lofi--param1-00.81.dac</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -873,9 +807,8 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="D25" t="inlineStr"/>
+        <v>0.8100000000000001</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -891,12 +824,11 @@
       <c r="C26" t="n">
         <v>0.91</v>
       </c>
-      <c r="D26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>lofi--param1-00.62--Cymatics.dac</t>
+          <t>lofi--param1-00.62.dac</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -907,7 +839,6 @@
       <c r="C27" t="n">
         <v>0.62</v>
       </c>
-      <c r="D27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -923,12 +854,11 @@
       <c r="C28" t="n">
         <v>0.93</v>
       </c>
-      <c r="D28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>lofi--param1-00.25--Cymatics.dac</t>
+          <t>lofi--param1-00.06.dac</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -937,9 +867,8 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="D29" t="inlineStr"/>
+        <v>0.06</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -955,12 +884,11 @@
       <c r="C30" t="n">
         <v>0.22</v>
       </c>
-      <c r="D30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>lofi--param1-00.14.dac</t>
+          <t>lofi--param1-00.58.dac</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -969,14 +897,13 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0.14</v>
-      </c>
-      <c r="D31" t="inlineStr"/>
+        <v>0.58</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>lofi--param1-00.06.dac</t>
+          <t>lofi--param1-00.02.dac</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -985,9 +912,8 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0.06</v>
-      </c>
-      <c r="D32" t="inlineStr"/>
+        <v>0.02</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1003,7 +929,6 @@
       <c r="C33" t="n">
         <v>0.92</v>
       </c>
-      <c r="D33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1019,12 +944,11 @@
       <c r="C34" t="n">
         <v>0.5</v>
       </c>
-      <c r="D34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>lofi--param1-00.02.dac</t>
+          <t>lofi--param1-00.01.dac</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1033,14 +957,13 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="D35" t="inlineStr"/>
+        <v>0.01</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>lofi--param1-00.01.dac</t>
+          <t>lofi--param1-00.14.dac</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1049,9 +972,8 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="D36" t="inlineStr"/>
+        <v>0.14</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1067,7 +989,6 @@
       <c r="C37" t="n">
         <v>0.2</v>
       </c>
-      <c r="D37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1083,7 +1004,6 @@
       <c r="C38" t="n">
         <v>1</v>
       </c>
-      <c r="D38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1099,7 +1019,6 @@
       <c r="C39" t="n">
         <v>0.18</v>
       </c>
-      <c r="D39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1115,647 +1034,606 @@
       <c r="C40" t="n">
         <v>0.35</v>
       </c>
-      <c r="D40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Fusion--param1-00.25.dac</t>
+          <t>8bit--param1-00.15.dac</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Fusion</t>
+          <t>8bit</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="D41" t="inlineStr"/>
+        <v>0.15</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Fusion--param1-00.65.dac</t>
+          <t>8bit--param1-00.62.dac</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Fusion</t>
+          <t>8bit</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>0.65</v>
-      </c>
-      <c r="D42" t="inlineStr"/>
+        <v>0.62</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Fusion--param1-00.40.dac</t>
+          <t>8bit--param1-00.89.dac</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Fusion</t>
+          <t>8bit</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="D43" t="inlineStr"/>
+        <v>0.89</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Fusion--param1-00.22.dac</t>
+          <t>8bit--param1-00.06.dac</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Fusion</t>
+          <t>8bit</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>0.22</v>
-      </c>
-      <c r="D44" t="inlineStr"/>
+        <v>0.06</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Fusion--param1-00.09.dac</t>
+          <t>8bit--param1-00.54.dac</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Fusion</t>
+          <t>8bit</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>0.09</v>
-      </c>
-      <c r="D45" t="inlineStr"/>
+        <v>0.54</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Fusion--param1-00.96--segment_03..dac</t>
+          <t>8bit--param1-00.08.dac</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Fusion</t>
+          <t>8bit</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>0.96</v>
-      </c>
-      <c r="D46" t="inlineStr"/>
+        <v>0.08</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Fusion--param1-00.24.dac</t>
+          <t>8bit--param1-00.55.dac</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Fusion</t>
+          <t>8bit</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>0.24</v>
-      </c>
-      <c r="D47" t="inlineStr"/>
+        <v>0.55</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Fusion--param1-00.20.dac</t>
+          <t>8bit--param1-00.60.dac</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Fusion</t>
+          <t>8bit</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="D48" t="inlineStr"/>
+        <v>0.6</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Fusion--param1-00.51.dac</t>
+          <t>8bit--param1-00.48.dac</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Fusion</t>
+          <t>8bit</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>0.51</v>
-      </c>
-      <c r="D49" t="inlineStr"/>
+        <v>0.48</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Fusion--param1-00.27.dac</t>
+          <t>8bit--param1-00.28.dac</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Fusion</t>
+          <t>8bit</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>0.27</v>
-      </c>
-      <c r="D50" t="inlineStr"/>
+        <v>0.28</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Fusion--param1-00.78.dac</t>
+          <t>8bit--param1-00.46.dac</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Fusion</t>
+          <t>8bit</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>0.78</v>
-      </c>
-      <c r="D51" t="inlineStr"/>
+        <v>0.46</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Fusion--param1-00.11.dac</t>
+          <t>8bit--param1-00.34.dac</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Fusion</t>
+          <t>8bit</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>0.11</v>
-      </c>
-      <c r="D52" t="inlineStr"/>
+        <v>0.34</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Fusion--param1-00.45.dac</t>
+          <t>8bit--param1-00.40.dac</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Fusion</t>
+          <t>8bit</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>0.45</v>
-      </c>
-      <c r="D53" t="inlineStr"/>
+        <v>0.4</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Fusion--param1-00.37.dac</t>
+          <t>8bit--param1-00.26.dac</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Fusion</t>
+          <t>8bit</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>0.37</v>
-      </c>
-      <c r="D54" t="inlineStr"/>
+        <v>0.26</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Fusion--param1-00.92--segment_09..dac</t>
+          <t>8bit--param1-00.67.dac</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Fusion</t>
+          <t>8bit</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>0.92</v>
-      </c>
-      <c r="D55" t="inlineStr"/>
+        <v>0.67</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Fusion--param1-00.79.dac</t>
+          <t>8bit--param1-00.96.dac</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Fusion</t>
+          <t>8bit</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>0.79</v>
-      </c>
-      <c r="D56" t="inlineStr"/>
+        <v>0.96</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Fusion--param1-00.34--segment_03..dac</t>
+          <t>8bit--param1-00.79.dac</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Fusion</t>
+          <t>8bit</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>0.34</v>
-      </c>
-      <c r="D57" t="inlineStr"/>
+        <v>0.79</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Fusion--param1-00.42.dac</t>
+          <t>8bit--param1-00.78.dac</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Fusion</t>
+          <t>8bit</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>0.42</v>
-      </c>
-      <c r="D58" t="inlineStr"/>
+        <v>0.78</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Fusion--param1-00.53.dac</t>
+          <t>8bit--param1-00.14.dac</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Fusion</t>
+          <t>8bit</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>0.53</v>
-      </c>
-      <c r="D59" t="inlineStr"/>
+        <v>0.14</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Fusion--param1-00.82.dac</t>
+          <t>8bit--param1-00.44.dac</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Fusion</t>
+          <t>8bit</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>0.82</v>
-      </c>
-      <c r="D60" t="inlineStr"/>
+        <v>0.44</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>8bit--param1-00.19--40.dac</t>
+          <t>Fusion--param1-00.09.dac</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>8bit</t>
+          <t>Fusion</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>0.19</v>
-      </c>
-      <c r="D61" t="inlineStr"/>
+        <v>0.09</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>8bit--param1-00.62--23.dac</t>
+          <t>Fusion--param1-00.67.dac</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>8bit</t>
+          <t>Fusion</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>0.62</v>
-      </c>
-      <c r="D62" t="inlineStr"/>
+        <v>0.67</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>8bit--param1-00.81.dac</t>
+          <t>Fusion--param1-00.41.dac</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>8bit</t>
+          <t>Fusion</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>0.8100000000000001</v>
-      </c>
-      <c r="D63" t="inlineStr"/>
+        <v>0.41</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>8bit--param1-00.01.dac</t>
+          <t>Fusion--param1-00.86.dac</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>8bit</t>
+          <t>Fusion</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="D64" t="inlineStr"/>
+        <v>0.86</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>8bit--param1-00.50.dac</t>
+          <t>Fusion--param1-00.36.dac</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>8bit</t>
+          <t>Fusion</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="D65" t="inlineStr"/>
+        <v>0.36</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>8bit--param1-00.55.dac</t>
+          <t>Fusion--param1-00.65.dac</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>8bit</t>
+          <t>Fusion</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>0.55</v>
-      </c>
-      <c r="D66" t="inlineStr"/>
+        <v>0.65</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>8bit--param1-00.85.dac</t>
+          <t>Fusion--param1-00.35.dac</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>8bit</t>
+          <t>Fusion</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>0.85</v>
-      </c>
-      <c r="D67" t="inlineStr"/>
+        <v>0.35</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>8bit--param1-00.71--31.dac</t>
+          <t>Fusion--param1-00.22.dac</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>8bit</t>
+          <t>Fusion</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>0.71</v>
-      </c>
-      <c r="D68" t="inlineStr"/>
+        <v>0.22</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>8bit--param1-00.15--43.dac</t>
+          <t>Fusion--param1-00.78.dac</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>8bit</t>
+          <t>Fusion</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="D69" t="inlineStr"/>
+        <v>0.78</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>8bit--param1-00.60.dac</t>
+          <t>Fusion--param1-00.24.dac</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>8bit</t>
+          <t>Fusion</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="D70" t="inlineStr"/>
+        <v>0.24</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>8bit--param1-00.06.dac</t>
+          <t>Fusion--param1-00.53.dac</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>8bit</t>
+          <t>Fusion</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>0.06</v>
-      </c>
-      <c r="D71" t="inlineStr"/>
+        <v>0.53</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>8bit--param1-00.14.dac</t>
+          <t>Fusion--param1-00.27.dac</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>8bit</t>
+          <t>Fusion</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>0.14</v>
-      </c>
-      <c r="D72" t="inlineStr"/>
+        <v>0.27</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>8bit--param1-00.62--01.dac</t>
+          <t>Fusion--param1-00.91.dac</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>8bit</t>
+          <t>Fusion</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>0.62</v>
-      </c>
-      <c r="D73" t="inlineStr"/>
+        <v>0.91</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>8bit--param1-00.88.dac</t>
+          <t>Fusion--param1-00.92.dac</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>8bit</t>
+          <t>Fusion</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>0.88</v>
-      </c>
-      <c r="D74" t="inlineStr"/>
+        <v>0.92</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>8bit--param1-00.82.dac</t>
+          <t>Fusion--param1-00.25.dac</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>8bit</t>
+          <t>Fusion</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>0.82</v>
-      </c>
-      <c r="D75" t="inlineStr"/>
+        <v>0.25</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>8bit--param1-00.67--19.dac</t>
+          <t>Fusion--param1-00.45.dac</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>8bit</t>
+          <t>Fusion</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>0.67</v>
-      </c>
-      <c r="D76" t="inlineStr"/>
+        <v>0.45</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>8bit--param1-00.49.dac</t>
+          <t>Fusion--param1-00.76.dac</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>8bit</t>
+          <t>Fusion</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>0.49</v>
-      </c>
-      <c r="D77" t="inlineStr"/>
+        <v>0.76</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>8bit--param1-00.40.dac</t>
+          <t>Fusion--param1-00.97.dac</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>8bit</t>
+          <t>Fusion</t>
         </is>
       </c>
       <c r="C78" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="D78" t="inlineStr"/>
+        <v>0.97</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>8bit--param1-00.71--46.dac</t>
+          <t>Fusion--param1-00.81.dac</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>8bit</t>
+          <t>Fusion</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>0.71</v>
-      </c>
-      <c r="D79" t="inlineStr"/>
+        <v>0.8100000000000001</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>8bit--param1-00.12.dac</t>
+          <t>Fusion--param1-00.96.dac</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>8bit</t>
+          <t>Fusion</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>0.12</v>
-      </c>
-      <c r="D80" t="inlineStr"/>
+        <v>0.96</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -1771,7 +1649,6 @@
       <c r="C81" t="n">
         <v>0.22</v>
       </c>
-      <c r="D81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -1787,12 +1664,11 @@
       <c r="C82" t="n">
         <v>0.51</v>
       </c>
-      <c r="D82" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>duduk--param1-00.77.dac</t>
+          <t>duduk--param1-00.88.dac</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -1801,9 +1677,8 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>0.77</v>
-      </c>
-      <c r="D83" t="inlineStr"/>
+        <v>0.88</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -1819,12 +1694,11 @@
       <c r="C84" t="n">
         <v>0.85</v>
       </c>
-      <c r="D84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>duduk--param1-00.70.dac</t>
+          <t>duduk--param1-00.67.dac</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -1833,14 +1707,13 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="D85" t="inlineStr"/>
+        <v>0.67</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>duduk--param1-00.11.dac</t>
+          <t>duduk--param1-00.76.dac</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -1849,14 +1722,13 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>0.11</v>
-      </c>
-      <c r="D86" t="inlineStr"/>
+        <v>0.76</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>duduk--param1-00.38.dac</t>
+          <t>duduk--param1-00.05.dac</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -1865,9 +1737,8 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>0.38</v>
-      </c>
-      <c r="D87" t="inlineStr"/>
+        <v>0.05</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -1883,12 +1754,11 @@
       <c r="C88" t="n">
         <v>0.55</v>
       </c>
-      <c r="D88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>duduk--param1-00.66.dac</t>
+          <t>duduk--param1-00.80.dac</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -1897,14 +1767,13 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>0.66</v>
-      </c>
-      <c r="D89" t="inlineStr"/>
+        <v>0.8</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>duduk--param1-00.88.dac</t>
+          <t>duduk--param1-00.74.dac</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
@@ -1913,9 +1782,8 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>0.88</v>
-      </c>
-      <c r="D90" t="inlineStr"/>
+        <v>0.74</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -1931,12 +1799,11 @@
       <c r="C91" t="n">
         <v>0.02</v>
       </c>
-      <c r="D91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>duduk--param1-00.80.dac</t>
+          <t>duduk--param1-00.54.dac</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
@@ -1945,14 +1812,13 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="D92" t="inlineStr"/>
+        <v>0.54</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>duduk--param1-00.54--KSHMR_Duduk_14_One_Shot_Fm.dac</t>
+          <t>duduk--param1-00.53.dac</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
@@ -1961,9 +1827,8 @@
         </is>
       </c>
       <c r="C93" t="n">
-        <v>0.54</v>
-      </c>
-      <c r="D93" t="inlineStr"/>
+        <v>0.53</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -1979,12 +1844,11 @@
       <c r="C94" t="n">
         <v>0.26</v>
       </c>
-      <c r="D94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>duduk--param1-00.58.dac</t>
+          <t>duduk--param1-00.70.dac</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
@@ -1993,14 +1857,13 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>0.58</v>
-      </c>
-      <c r="D95" t="inlineStr"/>
+        <v>0.7</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>duduk--param1-00.63.dac</t>
+          <t>duduk--param1-00.77.dac</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
@@ -2009,9 +1872,8 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>0.63</v>
-      </c>
-      <c r="D96" t="inlineStr"/>
+        <v>0.77</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -2027,12 +1889,11 @@
       <c r="C97" t="n">
         <v>0.23</v>
       </c>
-      <c r="D97" t="inlineStr"/>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>duduk--param1-00.74.dac</t>
+          <t>duduk--param1-00.58.dac</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
@@ -2041,9 +1902,8 @@
         </is>
       </c>
       <c r="C98" t="n">
-        <v>0.74</v>
-      </c>
-      <c r="D98" t="inlineStr"/>
+        <v>0.58</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -2059,12 +1919,11 @@
       <c r="C99" t="n">
         <v>0.93</v>
       </c>
-      <c r="D99" t="inlineStr"/>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>duduk--param1-00.76.dac</t>
+          <t>duduk--param1-00.63.dac</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -2073,9 +1932,8 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>0.76</v>
-      </c>
-      <c r="D100" t="inlineStr"/>
+        <v>0.63</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
add updated excels for dac train and val splits
</commit_message>
<xml_diff>
--- a/data/dac-train.xlsx
+++ b/data/dac-train.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C100"/>
+  <dimension ref="A1:D81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,611 +449,732 @@
           <t>Param1</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Param2</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Zelda--param1-00.11.dac</t>
+          <t>zelda--param1-00.23--5-06 Flight Range.dac</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Zelda</t>
+          <t>zelda</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.11</v>
+        <v>0.23</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>06 Flight Range</t>
+        </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Zelda--param1-00.16.dac</t>
+          <t>zelda--param1-00.28--6-10 Hyrule Castle.dac</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Zelda</t>
+          <t>zelda</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.16</v>
+        <v>0.28</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>10 Hyrule Castle</t>
+        </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Zelda--param1-00.19.dac</t>
+          <t>zelda--param1-00.02--2-25 Mipha's Role.dac</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Zelda</t>
+          <t>zelda</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.19</v>
+        <v>0.02</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>25 Mipha's Role</t>
+        </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Zelda--param1-00.40.dac</t>
+          <t>zelda--param1-00.83--2-34 Race Start.dac</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Zelda</t>
+          <t>zelda</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.4</v>
+        <v>0.83</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>34 Race Start</t>
+        </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Zelda--param1-00.48.dac</t>
+          <t>zelda--param1-00.66--6-15 Scourge of Hyrule Castle, Calamity Ganon Battle.dac</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Zelda</t>
+          <t>zelda</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.48</v>
+        <v>0.66</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>15 Scourge of Hyrule Castle, Calamity Ganon Battle</t>
+        </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Zelda--param1-00.03.dac</t>
+          <t>zelda--param1-00.72--4-19 Divine Beast, Vah Rudania Battle.dac</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Zelda</t>
+          <t>zelda</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.03</v>
+        <v>0.72</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>19 Divine Beast, Vah Rudania Battle</t>
+        </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Zelda--param1-00.04.dac</t>
+          <t>zelda--param1-00.46--5-07 Flight Range.dac</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Zelda</t>
+          <t>zelda</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.04</v>
+        <v>0.46</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>07 Flight Range</t>
+        </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Zelda--param1-00.30.dac</t>
+          <t>zelda--param1-00.71--2-12 Prince of Zoras, Sidon.dac</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Zelda</t>
+          <t>zelda</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.3</v>
+        <v>0.71</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>12 Prince of Zoras, Sidon</t>
+        </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Zelda--param1-00.14.dac</t>
+          <t>zelda--param1-00.91--2-40 Trophy Get.dac</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Zelda</t>
+          <t>zelda</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.14</v>
+        <v>0.91</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>40 Trophy Get</t>
+        </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Zelda--param1-00.18.dac</t>
+          <t>zelda--param1-00.69--6-17 Staff Roll.dac</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Zelda</t>
+          <t>zelda</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.18</v>
+        <v>0.6899999999999999</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>17 Staff Roll</t>
+        </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Zelda--param1-00.81.dac</t>
+          <t>zelda--param1-00.65--2-17 Link's Memories- Mipha's Touch.dac</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Zelda</t>
+          <t>zelda</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.65</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>17 Link's Memories- Mipha's Touch</t>
+        </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Zelda--param1-00.29.dac</t>
+          <t>zelda--param1-00.46--1-21 Calamity Ganon.dac</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Zelda</t>
+          <t>zelda</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.29</v>
+        <v>0.46</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>21 Calamity Ganon</t>
+        </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Zelda--param1-00.59.dac</t>
+          <t>zelda--param1-00.80--5-23 Battle (Strong Enemy).dac</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Zelda</t>
+          <t>zelda</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.59</v>
+        <v>0.8</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>23 Battle (Strong Enemy)</t>
+        </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Zelda--param1-00.34.dac</t>
+          <t>zelda--param1-00.05--1-09 The Beast.dac</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Zelda</t>
+          <t>zelda</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.34</v>
+        <v>0.05</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>09 The Beast</t>
+        </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Zelda--param1-00.75.dac</t>
+          <t>zelda--param1-00.12--2-28 Link's Memories - Slumbering Power.dac</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Zelda</t>
+          <t>zelda</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0.75</v>
+        <v>0.12</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>28 Link's Memories - Slumbering Power</t>
+        </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Zelda--param1-00.62.dac</t>
+          <t>zelda--param1-00.02--5-20 The Dragons of Hyrule.dac</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Zelda</t>
+          <t>zelda</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.62</v>
+        <v>0.02</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>20 The Dragons of Hyrule</t>
+        </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Zelda--param1-00.67.dac</t>
+          <t>zelda--param1-00.25--5-14 Rito Champion, Revali.dac</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Zelda</t>
+          <t>zelda</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.67</v>
+        <v>0.25</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>14 Rito Champion, Revali</t>
+        </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Zelda--param1-00.54.dac</t>
+          <t>zelda--param1-00.29.dac</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Zelda</t>
+          <t>zelda</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0.54</v>
-      </c>
+        <v>0.29</v>
+      </c>
+      <c r="D19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Zelda--param1-00.87.dac</t>
+          <t>zelda--param1-00.89--4-13 Divine Beast of the Volcano.dac</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Zelda</t>
+          <t>zelda</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0.87</v>
+        <v>0.89</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>13 Divine Beast of the Volcano</t>
+        </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Zelda--param1-00.37.dac</t>
+          <t>zelda--param1-00.86--3-12 Master Kohga's Theme.dac</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Zelda</t>
+          <t>zelda</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0.37</v>
+        <v>0.86</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>12 Master Kohga's Theme</t>
+        </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>lofi--param1-00.74.dac</t>
+          <t>fusion--param1-00.40--05. Rising.dac</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>lofi</t>
+          <t>fusion</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0.74</v>
-      </c>
+        <v>0.4</v>
+      </c>
+      <c r="D22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>lofi--param1-00.54.dac</t>
+          <t>fusion--param1-00.50--09. The Chieftain.dac</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>lofi</t>
+          <t>fusion</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0.54</v>
-      </c>
+        <v>0.5</v>
+      </c>
+      <c r="D23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>lofi--param1-00.38.dac</t>
+          <t>fusion--param1-00.95.dac</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>lofi</t>
+          <t>fusion</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.38</v>
-      </c>
+        <v>0.95</v>
+      </c>
+      <c r="D24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>lofi--param1-00.81.dac</t>
+          <t>fusion--param1-00.26.dac</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>lofi</t>
+          <t>fusion</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0.8100000000000001</v>
-      </c>
+        <v>0.26</v>
+      </c>
+      <c r="D25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>lofi--param1-00.91.dac</t>
+          <t>fusion--param1-00.94--09. The Chieftain.dac</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>lofi</t>
+          <t>fusion</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0.91</v>
-      </c>
+        <v>0.9399999999999999</v>
+      </c>
+      <c r="D26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>lofi--param1-00.62.dac</t>
+          <t>fusion--param1-00.08--01. The End.dac</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>lofi</t>
+          <t>fusion</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>0.62</v>
-      </c>
+        <v>0.08</v>
+      </c>
+      <c r="D27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>lofi--param1-00.93.dac</t>
+          <t>fusion--param1-00.39.dac</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>lofi</t>
+          <t>fusion</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>0.93</v>
-      </c>
+        <v>0.39</v>
+      </c>
+      <c r="D28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>lofi--param1-00.06.dac</t>
+          <t>fusion--param1-00.50--10. Rangda.dac</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>lofi</t>
+          <t>fusion</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>0.06</v>
-      </c>
+        <v>0.5</v>
+      </c>
+      <c r="D29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>lofi--param1-00.22.dac</t>
+          <t>fusion--param1-00.52.dac</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>lofi</t>
+          <t>fusion</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>0.22</v>
-      </c>
+        <v>0.52</v>
+      </c>
+      <c r="D30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>lofi--param1-00.58.dac</t>
+          <t>fusion--param1-00.61.dac</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>lofi</t>
+          <t>fusion</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0.58</v>
-      </c>
+        <v>0.61</v>
+      </c>
+      <c r="D31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>lofi--param1-00.02.dac</t>
+          <t>fusion--param1-00.86.dac</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>lofi</t>
+          <t>fusion</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0.02</v>
-      </c>
+        <v>0.86</v>
+      </c>
+      <c r="D32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>lofi--param1-00.92.dac</t>
+          <t>fusion--param1-00.46--04. Enter Rajasthan.dac</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>lofi</t>
+          <t>fusion</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>0.92</v>
-      </c>
+        <v>0.46</v>
+      </c>
+      <c r="D33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>lofi--param1-00.50.dac</t>
+          <t>fusion--param1-00.31.dac</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>lofi</t>
+          <t>fusion</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>0.5</v>
-      </c>
+        <v>0.31</v>
+      </c>
+      <c r="D34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>lofi--param1-00.01.dac</t>
+          <t>fusion--param1-00.46--03. All Gods With Me.dac</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>lofi</t>
+          <t>fusion</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>0.01</v>
-      </c>
+        <v>0.46</v>
+      </c>
+      <c r="D35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>lofi--param1-00.14.dac</t>
+          <t>fusion--param1-00.40--02. Lament.dac</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>lofi</t>
+          <t>fusion</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>0.14</v>
-      </c>
+        <v>0.4</v>
+      </c>
+      <c r="D36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>lofi--param1-00.20.dac</t>
+          <t>fusion--param1-00.45.dac</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>lofi</t>
+          <t>fusion</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>0.2</v>
-      </c>
+        <v>0.45</v>
+      </c>
+      <c r="D37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>lofi--param1-01.00.dac</t>
+          <t>fusion--param1-00.65.dac</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>lofi</t>
+          <t>fusion</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>1</v>
-      </c>
+        <v>0.65</v>
+      </c>
+      <c r="D38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>lofi--param1-00.18.dac</t>
+          <t>fusion--param1-00.33.dac</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>lofi</t>
+          <t>fusion</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>0.18</v>
-      </c>
+        <v>0.33</v>
+      </c>
+      <c r="D39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>lofi--param1-00.35.dac</t>
+          <t>fusion--param1-00.93.dac</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>lofi</t>
+          <t>fusion</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>0.35</v>
-      </c>
+        <v>0.93</v>
+      </c>
+      <c r="D40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>8bit--param1-00.15.dac</t>
+          <t>fusion--param1-00.15.dac</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>8bit</t>
+          <t>fusion</t>
         </is>
       </c>
       <c r="C41" t="n">
         <v>0.15</v>
       </c>
+      <c r="D41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>8bit--param1-00.62.dac</t>
+          <t>8bit--param1-00.12.dac</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1062,13 +1183,14 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>0.62</v>
-      </c>
+        <v>0.12</v>
+      </c>
+      <c r="D42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>8bit--param1-00.89.dac</t>
+          <t>8bit--param1-00.59.dac</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -1077,13 +1199,14 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>0.89</v>
-      </c>
+        <v>0.59</v>
+      </c>
+      <c r="D43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>8bit--param1-00.06.dac</t>
+          <t>8bit--param1-00.41.dac</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -1092,13 +1215,14 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>0.06</v>
-      </c>
+        <v>0.41</v>
+      </c>
+      <c r="D44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>8bit--param1-00.54.dac</t>
+          <t>8bit--param1-00.05.dac</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -1107,13 +1231,14 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>0.54</v>
-      </c>
+        <v>0.05</v>
+      </c>
+      <c r="D45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>8bit--param1-00.08.dac</t>
+          <t>8bit--param1-00.91.dac</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -1122,13 +1247,14 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>0.08</v>
-      </c>
+        <v>0.91</v>
+      </c>
+      <c r="D46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>8bit--param1-00.55.dac</t>
+          <t>8bit--param1-00.20.dac</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -1137,13 +1263,14 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>0.55</v>
-      </c>
+        <v>0.2</v>
+      </c>
+      <c r="D47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>8bit--param1-00.60.dac</t>
+          <t>8bit--param1-00.47.dac</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -1152,13 +1279,14 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>0.6</v>
-      </c>
+        <v>0.47</v>
+      </c>
+      <c r="D48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>8bit--param1-00.48.dac</t>
+          <t>8bit--param1-00.15--20 The Forest Guardian.dac</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -1167,13 +1295,14 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>0.48</v>
-      </c>
+        <v>0.15</v>
+      </c>
+      <c r="D49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>8bit--param1-00.28.dac</t>
+          <t>8bit--param1-00.28--09 Departure.dac</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -1184,11 +1313,12 @@
       <c r="C50" t="n">
         <v>0.28</v>
       </c>
+      <c r="D50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>8bit--param1-00.46.dac</t>
+          <t>8bit--param1-00.49.dac</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -1197,13 +1327,14 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>0.46</v>
-      </c>
+        <v>0.49</v>
+      </c>
+      <c r="D51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>8bit--param1-00.34.dac</t>
+          <t>8bit--param1-00.07.dac</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -1212,13 +1343,14 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>0.34</v>
-      </c>
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="D52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>8bit--param1-00.40.dac</t>
+          <t>8bit--param1-00.71--35 Moon Factory.dac</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -1227,13 +1359,14 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>0.4</v>
-      </c>
+        <v>0.71</v>
+      </c>
+      <c r="D53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>8bit--param1-00.26.dac</t>
+          <t>8bit--param1-00.90.dac</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -1242,13 +1375,14 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>0.26</v>
-      </c>
+        <v>0.9</v>
+      </c>
+      <c r="D54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>8bit--param1-00.67.dac</t>
+          <t>8bit--param1-00.62.dac</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -1257,13 +1391,14 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>0.67</v>
-      </c>
+        <v>0.62</v>
+      </c>
+      <c r="D55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>8bit--param1-00.96.dac</t>
+          <t>8bit--param1-00.25.dac</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1272,13 +1407,14 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>0.96</v>
-      </c>
+        <v>0.25</v>
+      </c>
+      <c r="D56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>8bit--param1-00.79.dac</t>
+          <t>8bit--param1-00.56.dac</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -1287,13 +1423,14 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>0.79</v>
-      </c>
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="D57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>8bit--param1-00.78.dac</t>
+          <t>8bit--param1-00.89.dac</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -1302,13 +1439,14 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>0.78</v>
-      </c>
+        <v>0.89</v>
+      </c>
+      <c r="D58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>8bit--param1-00.14.dac</t>
+          <t>8bit--param1-00.33.dac</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -1317,13 +1455,14 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>0.14</v>
-      </c>
+        <v>0.33</v>
+      </c>
+      <c r="D59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>8bit--param1-00.44.dac</t>
+          <t>8bit--param1-00.77.dac</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -1332,608 +1471,345 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>0.44</v>
-      </c>
+        <v>0.77</v>
+      </c>
+      <c r="D60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Fusion--param1-00.09.dac</t>
+          <t>8bit--param1-00.28--03 Ceremony.dac</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Fusion</t>
+          <t>8bit</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>0.09</v>
-      </c>
+        <v>0.28</v>
+      </c>
+      <c r="D61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Fusion--param1-00.67.dac</t>
+          <t>rock--param1-00.27--Power Rush.dac</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Fusion</t>
+          <t>rock</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>0.67</v>
-      </c>
+        <v>0.27</v>
+      </c>
+      <c r="D62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Fusion--param1-00.41.dac</t>
+          <t>rock--param1-00.02.dac</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Fusion</t>
+          <t>rock</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>0.41</v>
-      </c>
+        <v>0.02</v>
+      </c>
+      <c r="D63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Fusion--param1-00.86.dac</t>
+          <t>rock--param1-00.25.dac</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Fusion</t>
+          <t>rock</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>0.86</v>
-      </c>
+        <v>0.25</v>
+      </c>
+      <c r="D64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Fusion--param1-00.36.dac</t>
+          <t>rock--param1-00.18.dac</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Fusion</t>
+          <t>rock</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>0.36</v>
-      </c>
+        <v>0.18</v>
+      </c>
+      <c r="D65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Fusion--param1-00.65.dac</t>
+          <t>rock--param1-00.83.dac</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Fusion</t>
+          <t>rock</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>0.65</v>
-      </c>
+        <v>0.83</v>
+      </c>
+      <c r="D66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Fusion--param1-00.35.dac</t>
+          <t>rock--param1-00.28.dac</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Fusion</t>
+          <t>rock</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>0.35</v>
-      </c>
+        <v>0.28</v>
+      </c>
+      <c r="D67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Fusion--param1-00.22.dac</t>
+          <t>rock--param1-00.43.dac</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Fusion</t>
+          <t>rock</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>0.22</v>
-      </c>
+        <v>0.43</v>
+      </c>
+      <c r="D68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Fusion--param1-00.78.dac</t>
+          <t>rock--param1-00.40.dac</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Fusion</t>
+          <t>rock</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>0.78</v>
-      </c>
+        <v>0.4</v>
+      </c>
+      <c r="D69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Fusion--param1-00.24.dac</t>
+          <t>rock--param1-00.55.dac</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Fusion</t>
+          <t>rock</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>0.24</v>
-      </c>
+        <v>0.55</v>
+      </c>
+      <c r="D70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Fusion--param1-00.53.dac</t>
+          <t>rock--param1-00.73.dac</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Fusion</t>
+          <t>rock</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>0.53</v>
-      </c>
+        <v>0.73</v>
+      </c>
+      <c r="D71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Fusion--param1-00.27.dac</t>
+          <t>rock--param1-00.85.dac</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Fusion</t>
+          <t>rock</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>0.27</v>
-      </c>
+        <v>0.85</v>
+      </c>
+      <c r="D72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Fusion--param1-00.91.dac</t>
+          <t>rock--param1-00.62.dac</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Fusion</t>
+          <t>rock</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>0.91</v>
-      </c>
+        <v>0.62</v>
+      </c>
+      <c r="D73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Fusion--param1-00.92.dac</t>
+          <t>rock--param1-00.52.dac</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Fusion</t>
+          <t>rock</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>0.92</v>
-      </c>
+        <v>0.52</v>
+      </c>
+      <c r="D74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Fusion--param1-00.25.dac</t>
+          <t>rock--param1-00.97.dac</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Fusion</t>
+          <t>rock</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>0.25</v>
-      </c>
+        <v>0.97</v>
+      </c>
+      <c r="D75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Fusion--param1-00.45.dac</t>
+          <t>rock--param1-00.59.dac</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Fusion</t>
+          <t>rock</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>0.45</v>
-      </c>
+        <v>0.59</v>
+      </c>
+      <c r="D76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Fusion--param1-00.76.dac</t>
+          <t>rock--param1-00.78.dac</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Fusion</t>
+          <t>rock</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>0.76</v>
-      </c>
+        <v>0.78</v>
+      </c>
+      <c r="D77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Fusion--param1-00.97.dac</t>
+          <t>rock--param1-00.03.dac</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Fusion</t>
+          <t>rock</t>
         </is>
       </c>
       <c r="C78" t="n">
-        <v>0.97</v>
-      </c>
+        <v>0.03</v>
+      </c>
+      <c r="D78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Fusion--param1-00.81.dac</t>
+          <t>rock--param1-00.27--Go Ahead.dac</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Fusion</t>
+          <t>rock</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>0.8100000000000001</v>
-      </c>
+        <v>0.27</v>
+      </c>
+      <c r="D79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Fusion--param1-00.96.dac</t>
+          <t>rock--param1-00.20.dac</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Fusion</t>
+          <t>rock</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>0.96</v>
-      </c>
+        <v>0.2</v>
+      </c>
+      <c r="D80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>duduk--param1-00.22.dac</t>
+          <t>rock--param1-00.44.dac</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>duduk</t>
+          <t>rock</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>0.22</v>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="inlineStr">
-        <is>
-          <t>duduk--param1-00.51.dac</t>
-        </is>
-      </c>
-      <c r="B82" t="inlineStr">
-        <is>
-          <t>duduk</t>
-        </is>
-      </c>
-      <c r="C82" t="n">
-        <v>0.51</v>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="inlineStr">
-        <is>
-          <t>duduk--param1-00.88.dac</t>
-        </is>
-      </c>
-      <c r="B83" t="inlineStr">
-        <is>
-          <t>duduk</t>
-        </is>
-      </c>
-      <c r="C83" t="n">
-        <v>0.88</v>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="inlineStr">
-        <is>
-          <t>duduk--param1-00.85.dac</t>
-        </is>
-      </c>
-      <c r="B84" t="inlineStr">
-        <is>
-          <t>duduk</t>
-        </is>
-      </c>
-      <c r="C84" t="n">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="inlineStr">
-        <is>
-          <t>duduk--param1-00.67.dac</t>
-        </is>
-      </c>
-      <c r="B85" t="inlineStr">
-        <is>
-          <t>duduk</t>
-        </is>
-      </c>
-      <c r="C85" t="n">
-        <v>0.67</v>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="inlineStr">
-        <is>
-          <t>duduk--param1-00.76.dac</t>
-        </is>
-      </c>
-      <c r="B86" t="inlineStr">
-        <is>
-          <t>duduk</t>
-        </is>
-      </c>
-      <c r="C86" t="n">
-        <v>0.76</v>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="inlineStr">
-        <is>
-          <t>duduk--param1-00.05.dac</t>
-        </is>
-      </c>
-      <c r="B87" t="inlineStr">
-        <is>
-          <t>duduk</t>
-        </is>
-      </c>
-      <c r="C87" t="n">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="inlineStr">
-        <is>
-          <t>duduk--param1-00.55.dac</t>
-        </is>
-      </c>
-      <c r="B88" t="inlineStr">
-        <is>
-          <t>duduk</t>
-        </is>
-      </c>
-      <c r="C88" t="n">
-        <v>0.55</v>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="inlineStr">
-        <is>
-          <t>duduk--param1-00.80.dac</t>
-        </is>
-      </c>
-      <c r="B89" t="inlineStr">
-        <is>
-          <t>duduk</t>
-        </is>
-      </c>
-      <c r="C89" t="n">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="inlineStr">
-        <is>
-          <t>duduk--param1-00.74.dac</t>
-        </is>
-      </c>
-      <c r="B90" t="inlineStr">
-        <is>
-          <t>duduk</t>
-        </is>
-      </c>
-      <c r="C90" t="n">
-        <v>0.74</v>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="inlineStr">
-        <is>
-          <t>duduk--param1-00.02.dac</t>
-        </is>
-      </c>
-      <c r="B91" t="inlineStr">
-        <is>
-          <t>duduk</t>
-        </is>
-      </c>
-      <c r="C91" t="n">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" t="inlineStr">
-        <is>
-          <t>duduk--param1-00.54.dac</t>
-        </is>
-      </c>
-      <c r="B92" t="inlineStr">
-        <is>
-          <t>duduk</t>
-        </is>
-      </c>
-      <c r="C92" t="n">
-        <v>0.54</v>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" t="inlineStr">
-        <is>
-          <t>duduk--param1-00.53.dac</t>
-        </is>
-      </c>
-      <c r="B93" t="inlineStr">
-        <is>
-          <t>duduk</t>
-        </is>
-      </c>
-      <c r="C93" t="n">
-        <v>0.53</v>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" t="inlineStr">
-        <is>
-          <t>duduk--param1-00.26.dac</t>
-        </is>
-      </c>
-      <c r="B94" t="inlineStr">
-        <is>
-          <t>duduk</t>
-        </is>
-      </c>
-      <c r="C94" t="n">
-        <v>0.26</v>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" t="inlineStr">
-        <is>
-          <t>duduk--param1-00.70.dac</t>
-        </is>
-      </c>
-      <c r="B95" t="inlineStr">
-        <is>
-          <t>duduk</t>
-        </is>
-      </c>
-      <c r="C95" t="n">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" t="inlineStr">
-        <is>
-          <t>duduk--param1-00.77.dac</t>
-        </is>
-      </c>
-      <c r="B96" t="inlineStr">
-        <is>
-          <t>duduk</t>
-        </is>
-      </c>
-      <c r="C96" t="n">
-        <v>0.77</v>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="inlineStr">
-        <is>
-          <t>duduk--param1-00.23.dac</t>
-        </is>
-      </c>
-      <c r="B97" t="inlineStr">
-        <is>
-          <t>duduk</t>
-        </is>
-      </c>
-      <c r="C97" t="n">
-        <v>0.23</v>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" t="inlineStr">
-        <is>
-          <t>duduk--param1-00.58.dac</t>
-        </is>
-      </c>
-      <c r="B98" t="inlineStr">
-        <is>
-          <t>duduk</t>
-        </is>
-      </c>
-      <c r="C98" t="n">
-        <v>0.58</v>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" t="inlineStr">
-        <is>
-          <t>duduk--param1-00.93.dac</t>
-        </is>
-      </c>
-      <c r="B99" t="inlineStr">
-        <is>
-          <t>duduk</t>
-        </is>
-      </c>
-      <c r="C99" t="n">
-        <v>0.93</v>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" t="inlineStr">
-        <is>
-          <t>duduk--param1-00.63.dac</t>
-        </is>
-      </c>
-      <c r="B100" t="inlineStr">
-        <is>
-          <t>duduk</t>
-        </is>
-      </c>
-      <c r="C100" t="n">
-        <v>0.63</v>
-      </c>
+        <v>0.44</v>
+      </c>
+      <c r="D81" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>